<commit_message>
Updating aggregate and recent data
</commit_message>
<xml_diff>
--- a/data/recent data/Recent_Data.xlsx
+++ b/data/recent data/Recent_Data.xlsx
@@ -229,7 +229,7 @@
     <t>San Diego Central Jail, George Bailey Detention Facility, East Mesa Re-Entry Facility, Vista Detention Facility, Las Colinas Detention and Re-Entry Facility, South Bay Detention Facility, and Facility 8 Detention Facility</t>
   </si>
   <si>
-    <t>Intake &amp; Release Center, Jail #2 and Jail #18</t>
+    <t>Intake &amp; Release Center, Jail #2 and Jail #3</t>
   </si>
   <si>
     <t>John J. Zunino Facility, San Joaquin County Honor Farm</t>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="2">
-        <v>45047</v>
+        <v>45092</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
@@ -1009,28 +1009,28 @@
         <v>89</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>2213</v>
+        <v>2216</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>37706</v>
+        <v>37870</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1766</v>
+        <v>1714</v>
       </c>
       <c r="N5">
-        <v>688</v>
+        <v>692</v>
       </c>
       <c r="O5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:38">
@@ -1810,7 +1810,7 @@
     </row>
     <row r="35" spans="1:36">
       <c r="A35" s="2">
-        <v>45048</v>
+        <v>45092</v>
       </c>
       <c r="B35" t="s">
         <v>52</v>
@@ -1819,13 +1819,13 @@
         <v>103</v>
       </c>
       <c r="D35">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="F35">
         <v>25</v>
       </c>
       <c r="I35">
-        <v>13689</v>
+        <v>13224</v>
       </c>
     </row>
     <row r="36" spans="1:36">
@@ -2621,7 +2621,7 @@
     </row>
     <row r="64" spans="1:36">
       <c r="A64" s="2">
-        <v>45047</v>
+        <v>45061</v>
       </c>
       <c r="B64" t="s">
         <v>63</v>
@@ -2630,16 +2630,16 @@
         <v>114</v>
       </c>
       <c r="D64">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E64">
-        <v>4124</v>
+        <v>4164</v>
       </c>
       <c r="G64">
-        <v>51299</v>
+        <v>51870</v>
       </c>
       <c r="H64">
-        <v>89</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:38">
@@ -2818,7 +2818,7 @@
     </row>
     <row r="74" spans="1:38">
       <c r="A74" s="2">
-        <v>45042</v>
+        <v>45070</v>
       </c>
       <c r="B74" t="s">
         <v>67</v>
@@ -2827,19 +2827,19 @@
         <v>118</v>
       </c>
       <c r="D74">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E74">
-        <v>4563</v>
+        <v>4569</v>
       </c>
       <c r="F74">
         <v>3</v>
       </c>
       <c r="G74">
-        <v>59379</v>
+        <v>59407</v>
       </c>
       <c r="I74">
-        <v>2994</v>
+        <v>2968</v>
       </c>
     </row>
     <row r="75" spans="1:38">
@@ -3111,7 +3111,7 @@
     </row>
     <row r="84" spans="1:36">
       <c r="A84" s="2">
-        <v>45042</v>
+        <v>45092</v>
       </c>
       <c r="B84" t="s">
         <v>70</v>
@@ -3120,13 +3120,13 @@
         <v>121</v>
       </c>
       <c r="AA84">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AB84">
         <v>3</v>
       </c>
       <c r="AC84">
-        <v>3423</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="85" spans="1:36">
@@ -3305,7 +3305,7 @@
     </row>
     <row r="94" spans="1:36">
       <c r="A94" s="2">
-        <v>45050</v>
+        <v>45055</v>
       </c>
       <c r="B94" t="s">
         <v>71</v>
@@ -3320,7 +3320,7 @@
         <v>694</v>
       </c>
       <c r="I94">
-        <v>836</v>
+        <v>857</v>
       </c>
     </row>
     <row r="95" spans="1:36">
@@ -3755,7 +3755,7 @@
     </row>
     <row r="112" spans="1:36">
       <c r="A112" s="2">
-        <v>45049</v>
+        <v>45092</v>
       </c>
       <c r="B112" t="s">
         <v>76</v>
@@ -3764,25 +3764,25 @@
         <v>127</v>
       </c>
       <c r="D112">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E112">
-        <v>2793</v>
+        <v>2833</v>
       </c>
       <c r="G112">
-        <v>90871</v>
+        <v>93133</v>
       </c>
       <c r="I112">
-        <v>2935</v>
+        <v>2926</v>
       </c>
       <c r="AA112">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AC112">
-        <v>1549</v>
+        <v>1566</v>
       </c>
       <c r="AD112">
-        <v>211671</v>
+        <v>216909</v>
       </c>
     </row>
     <row r="113" spans="1:36">

</xml_diff>